<commit_message>
Alteração documentação e correção validação login
</commit_message>
<xml_diff>
--- a/Documentos/Casos de teste e histórias de usuários.xlsx
+++ b/Documentos/Casos de teste e histórias de usuários.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cenários e casos de teste" sheetId="1" r:id="rId1"/>
     <sheet name="Histórias de usuários" sheetId="2" r:id="rId2"/>
+    <sheet name="Planilha1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="185">
   <si>
     <t>ID - Teste</t>
   </si>
@@ -574,13 +575,19 @@
   </si>
   <si>
     <t>Não foi implementada</t>
+  </si>
+  <si>
+    <t>Visualizar as estruturas que compõem o sistema locomotor bovino</t>
+  </si>
+  <si>
+    <t>Visualizar as imagens de uma parte específica da estrutura do esqueleto do boi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -617,8 +624,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -652,6 +666,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFBFBF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD966"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -769,7 +795,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -870,6 +896,33 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -882,6 +935,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -891,6 +947,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -900,40 +962,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1218,8 +1269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L249"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1236,11 +1287,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
     </row>
@@ -1259,19 +1310,19 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" s="55" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="53"/>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
+    <row r="3" spans="1:12" s="38" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="36"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
     </row>
     <row r="4" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1280,10 +1331,10 @@
       <c r="B4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="34" t="s">
         <v>129</v>
       </c>
-      <c r="D4" s="54"/>
+      <c r="D4" s="37"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1300,2188 +1351,2188 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="43" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="43" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
-      <c r="B8" s="34"/>
+      <c r="A8" s="42"/>
+      <c r="B8" s="43"/>
       <c r="C8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="34"/>
+      <c r="D8" s="43"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
-      <c r="B9" s="34"/>
+      <c r="A9" s="42"/>
+      <c r="B9" s="43"/>
       <c r="C9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="34"/>
+      <c r="D9" s="43"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="43" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="43" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
-      <c r="B11" s="34"/>
+      <c r="A11" s="42"/>
+      <c r="B11" s="43"/>
       <c r="C11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="34"/>
+      <c r="D11" s="43"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
-      <c r="B12" s="34"/>
+      <c r="A12" s="42"/>
+      <c r="B12" s="43"/>
       <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="34"/>
+      <c r="D12" s="43"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
-      <c r="B13" s="34"/>
+      <c r="A13" s="42"/>
+      <c r="B13" s="43"/>
       <c r="C13" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="34"/>
+      <c r="D13" s="43"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="47" t="s">
+      <c r="A14" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="42" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="34" t="s">
+      <c r="D14" s="43" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="48"/>
-      <c r="B15" s="44"/>
+      <c r="A15" s="40"/>
+      <c r="B15" s="42"/>
       <c r="C15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="34"/>
+      <c r="D15" s="43"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="48"/>
-      <c r="B16" s="44"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="34"/>
+      <c r="D16" s="43"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="48"/>
-      <c r="B17" s="44"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="34"/>
+      <c r="D17" s="43"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="49"/>
-      <c r="B18" s="44"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="34"/>
+      <c r="D18" s="43"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="43" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="35" t="s">
+      <c r="D19" s="44" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
-      <c r="B20" s="34"/>
+      <c r="A20" s="42"/>
+      <c r="B20" s="43"/>
       <c r="C20" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="36"/>
+      <c r="D20" s="45"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="44"/>
-      <c r="B21" s="34"/>
+      <c r="A21" s="42"/>
+      <c r="B21" s="43"/>
       <c r="C21" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="36"/>
+      <c r="D21" s="45"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
-      <c r="B22" s="34"/>
+      <c r="A22" s="42"/>
+      <c r="B22" s="43"/>
       <c r="C22" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="37"/>
+      <c r="D22" s="46"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="47" t="s">
+      <c r="A23" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="42" t="s">
         <v>16</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="34" t="s">
+      <c r="D23" s="43" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="48"/>
-      <c r="B24" s="44"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="42"/>
       <c r="C24" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="34"/>
+      <c r="D24" s="43"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="48"/>
-      <c r="B25" s="44"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="42"/>
       <c r="C25" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="34"/>
+      <c r="D25" s="43"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="48"/>
-      <c r="B26" s="44"/>
+      <c r="A26" s="40"/>
+      <c r="B26" s="42"/>
       <c r="C26" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="34"/>
+      <c r="D26" s="43"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="49"/>
-      <c r="B27" s="44"/>
+      <c r="A27" s="41"/>
+      <c r="B27" s="42"/>
       <c r="C27" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="34"/>
+      <c r="D27" s="43"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="44" t="s">
+      <c r="A28" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="34" t="s">
+      <c r="B28" s="43" t="s">
         <v>16</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="35" t="s">
+      <c r="D28" s="44" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
-      <c r="B29" s="34"/>
+      <c r="A29" s="42"/>
+      <c r="B29" s="43"/>
       <c r="C29" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="36"/>
+      <c r="D29" s="45"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
-      <c r="B30" s="34"/>
+      <c r="A30" s="42"/>
+      <c r="B30" s="43"/>
       <c r="C30" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="36"/>
+      <c r="D30" s="45"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="44"/>
-      <c r="B31" s="34"/>
+      <c r="A31" s="42"/>
+      <c r="B31" s="43"/>
       <c r="C31" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="37"/>
+      <c r="D31" s="46"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="47" t="s">
+      <c r="A32" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="44" t="s">
+      <c r="B32" s="42" t="s">
         <v>16</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="34" t="s">
+      <c r="D32" s="43" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="48"/>
-      <c r="B33" s="44"/>
+      <c r="A33" s="40"/>
+      <c r="B33" s="42"/>
       <c r="C33" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D33" s="34"/>
+      <c r="D33" s="43"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="48"/>
-      <c r="B34" s="44"/>
+      <c r="A34" s="40"/>
+      <c r="B34" s="42"/>
       <c r="C34" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D34" s="34"/>
+      <c r="D34" s="43"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="48"/>
-      <c r="B35" s="44"/>
+      <c r="A35" s="40"/>
+      <c r="B35" s="42"/>
       <c r="C35" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D35" s="34"/>
+      <c r="D35" s="43"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="49"/>
-      <c r="B36" s="44"/>
+      <c r="A36" s="41"/>
+      <c r="B36" s="42"/>
       <c r="C36" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D36" s="34"/>
+      <c r="D36" s="43"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="44" t="s">
+      <c r="A37" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="B37" s="34" t="s">
+      <c r="B37" s="43" t="s">
         <v>16</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D37" s="35" t="s">
+      <c r="D37" s="44" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="44"/>
-      <c r="B38" s="34"/>
+      <c r="A38" s="42"/>
+      <c r="B38" s="43"/>
       <c r="C38" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D38" s="36"/>
+      <c r="D38" s="45"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="44"/>
-      <c r="B39" s="34"/>
+      <c r="A39" s="42"/>
+      <c r="B39" s="43"/>
       <c r="C39" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D39" s="36"/>
+      <c r="D39" s="45"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="44"/>
-      <c r="B40" s="34"/>
+      <c r="A40" s="42"/>
+      <c r="B40" s="43"/>
       <c r="C40" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D40" s="37"/>
+      <c r="D40" s="46"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="47" t="s">
+      <c r="A41" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="44" t="s">
+      <c r="B41" s="42" t="s">
         <v>16</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D41" s="34" t="s">
+      <c r="D41" s="43" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="48"/>
-      <c r="B42" s="44"/>
+      <c r="A42" s="40"/>
+      <c r="B42" s="42"/>
       <c r="C42" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D42" s="34"/>
+      <c r="D42" s="43"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="48"/>
-      <c r="B43" s="44"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="42"/>
       <c r="C43" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D43" s="34"/>
+      <c r="D43" s="43"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="48"/>
-      <c r="B44" s="44"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="42"/>
       <c r="C44" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D44" s="34"/>
+      <c r="D44" s="43"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="49"/>
-      <c r="B45" s="44"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="42"/>
       <c r="C45" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D45" s="34"/>
+      <c r="D45" s="43"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="44" t="s">
+      <c r="A46" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="B46" s="34" t="s">
+      <c r="B46" s="43" t="s">
         <v>16</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D46" s="35" t="s">
+      <c r="D46" s="44" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="44"/>
-      <c r="B47" s="34"/>
+      <c r="A47" s="42"/>
+      <c r="B47" s="43"/>
       <c r="C47" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D47" s="36"/>
+      <c r="D47" s="45"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="44"/>
-      <c r="B48" s="34"/>
+      <c r="A48" s="42"/>
+      <c r="B48" s="43"/>
       <c r="C48" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D48" s="36"/>
+      <c r="D48" s="45"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="44"/>
-      <c r="B49" s="34"/>
+      <c r="A49" s="42"/>
+      <c r="B49" s="43"/>
       <c r="C49" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D49" s="37"/>
+      <c r="D49" s="46"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="47" t="s">
+      <c r="A50" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="B50" s="44" t="s">
+      <c r="B50" s="42" t="s">
         <v>16</v>
       </c>
       <c r="C50" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D50" s="34" t="s">
+      <c r="D50" s="43" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="48"/>
-      <c r="B51" s="44"/>
+      <c r="A51" s="40"/>
+      <c r="B51" s="42"/>
       <c r="C51" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D51" s="34"/>
+      <c r="D51" s="43"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="48"/>
-      <c r="B52" s="44"/>
+      <c r="A52" s="40"/>
+      <c r="B52" s="42"/>
       <c r="C52" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D52" s="34"/>
+      <c r="D52" s="43"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="48"/>
-      <c r="B53" s="44"/>
+      <c r="A53" s="40"/>
+      <c r="B53" s="42"/>
       <c r="C53" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D53" s="34"/>
+      <c r="D53" s="43"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="49"/>
-      <c r="B54" s="44"/>
+      <c r="A54" s="41"/>
+      <c r="B54" s="42"/>
       <c r="C54" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D54" s="34"/>
+      <c r="D54" s="43"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="44" t="s">
+      <c r="A55" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="B55" s="34" t="s">
+      <c r="B55" s="43" t="s">
         <v>16</v>
       </c>
       <c r="C55" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D55" s="34" t="s">
+      <c r="D55" s="43" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="44"/>
-      <c r="B56" s="34"/>
+      <c r="A56" s="42"/>
+      <c r="B56" s="43"/>
       <c r="C56" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D56" s="34"/>
+      <c r="D56" s="43"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="44"/>
-      <c r="B57" s="34"/>
+      <c r="A57" s="42"/>
+      <c r="B57" s="43"/>
       <c r="C57" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D57" s="34"/>
+      <c r="D57" s="43"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="44"/>
-      <c r="B58" s="34"/>
+      <c r="A58" s="42"/>
+      <c r="B58" s="43"/>
       <c r="C58" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D58" s="34"/>
+      <c r="D58" s="43"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="47" t="s">
+      <c r="A59" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="B59" s="44" t="s">
+      <c r="B59" s="42" t="s">
         <v>16</v>
       </c>
       <c r="C59" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D59" s="34" t="s">
+      <c r="D59" s="43" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="48"/>
-      <c r="B60" s="44"/>
+      <c r="A60" s="40"/>
+      <c r="B60" s="42"/>
       <c r="C60" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D60" s="34"/>
+      <c r="D60" s="43"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="48"/>
-      <c r="B61" s="44"/>
+      <c r="A61" s="40"/>
+      <c r="B61" s="42"/>
       <c r="C61" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D61" s="34"/>
+      <c r="D61" s="43"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="48"/>
-      <c r="B62" s="44"/>
+      <c r="A62" s="40"/>
+      <c r="B62" s="42"/>
       <c r="C62" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D62" s="34"/>
+      <c r="D62" s="43"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="49"/>
-      <c r="B63" s="44"/>
+      <c r="A63" s="41"/>
+      <c r="B63" s="42"/>
       <c r="C63" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D63" s="34"/>
+      <c r="D63" s="43"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="34" t="s">
+      <c r="A64" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="B64" s="34" t="s">
+      <c r="B64" s="43" t="s">
         <v>43</v>
       </c>
       <c r="C64" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D64" s="34" t="s">
+      <c r="D64" s="43" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="34"/>
-      <c r="B65" s="34"/>
+      <c r="A65" s="43"/>
+      <c r="B65" s="43"/>
       <c r="C65" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D65" s="34"/>
+      <c r="D65" s="43"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="34"/>
-      <c r="B66" s="34"/>
+      <c r="A66" s="43"/>
+      <c r="B66" s="43"/>
       <c r="C66" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D66" s="34"/>
+      <c r="D66" s="43"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="34"/>
-      <c r="B67" s="34"/>
+      <c r="A67" s="43"/>
+      <c r="B67" s="43"/>
       <c r="C67" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D67" s="34"/>
+      <c r="D67" s="43"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="34"/>
-      <c r="B68" s="34"/>
+      <c r="A68" s="43"/>
+      <c r="B68" s="43"/>
       <c r="C68" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D68" s="34"/>
+      <c r="D68" s="43"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="34" t="s">
+      <c r="A69" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="B69" s="34" t="s">
+      <c r="B69" s="43" t="s">
         <v>43</v>
       </c>
       <c r="C69" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D69" s="34" t="s">
+      <c r="D69" s="43" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="34"/>
-      <c r="B70" s="34"/>
+      <c r="A70" s="43"/>
+      <c r="B70" s="43"/>
       <c r="C70" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D70" s="34"/>
+      <c r="D70" s="43"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="34"/>
-      <c r="B71" s="34"/>
+      <c r="A71" s="43"/>
+      <c r="B71" s="43"/>
       <c r="C71" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D71" s="34"/>
+      <c r="D71" s="43"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="34"/>
-      <c r="B72" s="34"/>
+      <c r="A72" s="43"/>
+      <c r="B72" s="43"/>
       <c r="C72" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D72" s="34"/>
+      <c r="D72" s="43"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="34"/>
-      <c r="B73" s="34"/>
+      <c r="A73" s="43"/>
+      <c r="B73" s="43"/>
       <c r="C73" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D73" s="34"/>
+      <c r="D73" s="43"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="34" t="s">
+      <c r="A74" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="B74" s="34" t="s">
+      <c r="B74" s="43" t="s">
         <v>43</v>
       </c>
       <c r="C74" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D74" s="34" t="s">
+      <c r="D74" s="43" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="34"/>
-      <c r="B75" s="34"/>
+      <c r="A75" s="43"/>
+      <c r="B75" s="43"/>
       <c r="C75" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D75" s="34"/>
+      <c r="D75" s="43"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="34"/>
-      <c r="B76" s="34"/>
+      <c r="A76" s="43"/>
+      <c r="B76" s="43"/>
       <c r="C76" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D76" s="34"/>
+      <c r="D76" s="43"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="34"/>
-      <c r="B77" s="34"/>
+      <c r="A77" s="43"/>
+      <c r="B77" s="43"/>
       <c r="C77" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D77" s="34"/>
+      <c r="D77" s="43"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="34"/>
-      <c r="B78" s="34"/>
+      <c r="A78" s="43"/>
+      <c r="B78" s="43"/>
       <c r="C78" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D78" s="34"/>
+      <c r="D78" s="43"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="34" t="s">
+      <c r="A79" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="B79" s="34" t="s">
+      <c r="B79" s="43" t="s">
         <v>43</v>
       </c>
       <c r="C79" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D79" s="34" t="s">
+      <c r="D79" s="43" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="34"/>
-      <c r="B80" s="34"/>
+      <c r="A80" s="43"/>
+      <c r="B80" s="43"/>
       <c r="C80" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D80" s="34"/>
+      <c r="D80" s="43"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="34"/>
-      <c r="B81" s="34"/>
+      <c r="A81" s="43"/>
+      <c r="B81" s="43"/>
       <c r="C81" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D81" s="34"/>
+      <c r="D81" s="43"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="34"/>
-      <c r="B82" s="34"/>
+      <c r="A82" s="43"/>
+      <c r="B82" s="43"/>
       <c r="C82" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D82" s="34"/>
+      <c r="D82" s="43"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="34"/>
-      <c r="B83" s="34"/>
+      <c r="A83" s="43"/>
+      <c r="B83" s="43"/>
       <c r="C83" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D83" s="34"/>
+      <c r="D83" s="43"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="34" t="s">
+      <c r="A84" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="B84" s="34" t="s">
+      <c r="B84" s="43" t="s">
         <v>43</v>
       </c>
       <c r="C84" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D84" s="34" t="s">
+      <c r="D84" s="43" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="34"/>
-      <c r="B85" s="34"/>
+      <c r="A85" s="43"/>
+      <c r="B85" s="43"/>
       <c r="C85" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D85" s="34"/>
+      <c r="D85" s="43"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="34"/>
-      <c r="B86" s="34"/>
+      <c r="A86" s="43"/>
+      <c r="B86" s="43"/>
       <c r="C86" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D86" s="34"/>
+      <c r="D86" s="43"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="34"/>
-      <c r="B87" s="34"/>
+      <c r="A87" s="43"/>
+      <c r="B87" s="43"/>
       <c r="C87" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D87" s="34"/>
+      <c r="D87" s="43"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="34"/>
-      <c r="B88" s="34"/>
+      <c r="A88" s="43"/>
+      <c r="B88" s="43"/>
       <c r="C88" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D88" s="34"/>
+      <c r="D88" s="43"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="34" t="s">
+      <c r="A89" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="B89" s="34" t="s">
+      <c r="B89" s="43" t="s">
         <v>43</v>
       </c>
       <c r="C89" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D89" s="34" t="s">
+      <c r="D89" s="43" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="34"/>
-      <c r="B90" s="34"/>
+      <c r="A90" s="43"/>
+      <c r="B90" s="43"/>
       <c r="C90" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D90" s="34"/>
+      <c r="D90" s="43"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="34"/>
-      <c r="B91" s="34"/>
+      <c r="A91" s="43"/>
+      <c r="B91" s="43"/>
       <c r="C91" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D91" s="34"/>
+      <c r="D91" s="43"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="34"/>
-      <c r="B92" s="34"/>
+      <c r="A92" s="43"/>
+      <c r="B92" s="43"/>
       <c r="C92" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D92" s="34"/>
+      <c r="D92" s="43"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="34"/>
-      <c r="B93" s="34"/>
+      <c r="A93" s="43"/>
+      <c r="B93" s="43"/>
       <c r="C93" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D93" s="34"/>
+      <c r="D93" s="43"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="38" t="s">
+      <c r="A94" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="B94" s="35" t="s">
+      <c r="B94" s="44" t="s">
         <v>52</v>
       </c>
       <c r="C94" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D94" s="35" t="s">
+      <c r="D94" s="44" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="39"/>
-      <c r="B95" s="36"/>
+      <c r="A95" s="49"/>
+      <c r="B95" s="45"/>
       <c r="C95" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D95" s="36"/>
+      <c r="D95" s="45"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="39"/>
-      <c r="B96" s="36"/>
+      <c r="A96" s="49"/>
+      <c r="B96" s="45"/>
       <c r="C96" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D96" s="36"/>
+      <c r="D96" s="45"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="39"/>
-      <c r="B97" s="36"/>
+      <c r="A97" s="49"/>
+      <c r="B97" s="45"/>
       <c r="C97" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D97" s="36"/>
+      <c r="D97" s="45"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="40"/>
-      <c r="B98" s="37"/>
+      <c r="A98" s="50"/>
+      <c r="B98" s="46"/>
       <c r="C98" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D98" s="37"/>
+      <c r="D98" s="46"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="38" t="s">
+      <c r="A99" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="B99" s="35" t="s">
+      <c r="B99" s="44" t="s">
         <v>52</v>
       </c>
       <c r="C99" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D99" s="35" t="s">
+      <c r="D99" s="44" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="39"/>
-      <c r="B100" s="36"/>
+      <c r="A100" s="49"/>
+      <c r="B100" s="45"/>
       <c r="C100" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D100" s="36"/>
+      <c r="D100" s="45"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="39"/>
-      <c r="B101" s="36"/>
+      <c r="A101" s="49"/>
+      <c r="B101" s="45"/>
       <c r="C101" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D101" s="36"/>
+      <c r="D101" s="45"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="39"/>
-      <c r="B102" s="36"/>
+      <c r="A102" s="49"/>
+      <c r="B102" s="45"/>
       <c r="C102" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D102" s="36"/>
+      <c r="D102" s="45"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="40"/>
-      <c r="B103" s="37"/>
+      <c r="A103" s="50"/>
+      <c r="B103" s="46"/>
       <c r="C103" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D103" s="37"/>
+      <c r="D103" s="46"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="38" t="s">
+      <c r="A104" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="B104" s="35" t="s">
+      <c r="B104" s="44" t="s">
         <v>52</v>
       </c>
       <c r="C104" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D104" s="35" t="s">
+      <c r="D104" s="44" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="39"/>
-      <c r="B105" s="36"/>
+      <c r="A105" s="49"/>
+      <c r="B105" s="45"/>
       <c r="C105" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D105" s="36"/>
+      <c r="D105" s="45"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="39"/>
-      <c r="B106" s="36"/>
+      <c r="A106" s="49"/>
+      <c r="B106" s="45"/>
       <c r="C106" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D106" s="36"/>
+      <c r="D106" s="45"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="39"/>
-      <c r="B107" s="36"/>
+      <c r="A107" s="49"/>
+      <c r="B107" s="45"/>
       <c r="C107" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D107" s="36"/>
+      <c r="D107" s="45"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="40"/>
-      <c r="B108" s="37"/>
+      <c r="A108" s="50"/>
+      <c r="B108" s="46"/>
       <c r="C108" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D108" s="37"/>
+      <c r="D108" s="46"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="38" t="s">
+      <c r="A109" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="B109" s="35" t="s">
+      <c r="B109" s="44" t="s">
         <v>52</v>
       </c>
       <c r="C109" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D109" s="35" t="s">
+      <c r="D109" s="44" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="39"/>
-      <c r="B110" s="36"/>
+      <c r="A110" s="49"/>
+      <c r="B110" s="45"/>
       <c r="C110" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D110" s="36"/>
+      <c r="D110" s="45"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="39"/>
-      <c r="B111" s="36"/>
+      <c r="A111" s="49"/>
+      <c r="B111" s="45"/>
       <c r="C111" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D111" s="36"/>
+      <c r="D111" s="45"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="39"/>
-      <c r="B112" s="36"/>
+      <c r="A112" s="49"/>
+      <c r="B112" s="45"/>
       <c r="C112" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D112" s="36"/>
+      <c r="D112" s="45"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="40"/>
-      <c r="B113" s="37"/>
+      <c r="A113" s="50"/>
+      <c r="B113" s="46"/>
       <c r="C113" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D113" s="37"/>
+      <c r="D113" s="46"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="38" t="s">
+      <c r="A114" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="B114" s="35" t="s">
+      <c r="B114" s="44" t="s">
         <v>52</v>
       </c>
       <c r="C114" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D114" s="35" t="s">
+      <c r="D114" s="44" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="39"/>
-      <c r="B115" s="36"/>
+      <c r="A115" s="49"/>
+      <c r="B115" s="45"/>
       <c r="C115" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D115" s="36"/>
+      <c r="D115" s="45"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="39"/>
-      <c r="B116" s="36"/>
+      <c r="A116" s="49"/>
+      <c r="B116" s="45"/>
       <c r="C116" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D116" s="36"/>
+      <c r="D116" s="45"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="39"/>
-      <c r="B117" s="36"/>
+      <c r="A117" s="49"/>
+      <c r="B117" s="45"/>
       <c r="C117" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D117" s="36"/>
+      <c r="D117" s="45"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="40"/>
-      <c r="B118" s="37"/>
+      <c r="A118" s="50"/>
+      <c r="B118" s="46"/>
       <c r="C118" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D118" s="37"/>
+      <c r="D118" s="46"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="38" t="s">
+      <c r="A119" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="B119" s="35" t="s">
+      <c r="B119" s="44" t="s">
         <v>52</v>
       </c>
       <c r="C119" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D119" s="35" t="s">
+      <c r="D119" s="44" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="39"/>
-      <c r="B120" s="36"/>
+      <c r="A120" s="49"/>
+      <c r="B120" s="45"/>
       <c r="C120" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D120" s="36"/>
+      <c r="D120" s="45"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="39"/>
-      <c r="B121" s="36"/>
+      <c r="A121" s="49"/>
+      <c r="B121" s="45"/>
       <c r="C121" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D121" s="36"/>
+      <c r="D121" s="45"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="39"/>
-      <c r="B122" s="36"/>
+      <c r="A122" s="49"/>
+      <c r="B122" s="45"/>
       <c r="C122" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D122" s="36"/>
+      <c r="D122" s="45"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="40"/>
-      <c r="B123" s="37"/>
+      <c r="A123" s="50"/>
+      <c r="B123" s="46"/>
       <c r="C123" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D123" s="37"/>
+      <c r="D123" s="46"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="44" t="s">
+      <c r="A124" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="B124" s="34" t="s">
+      <c r="B124" s="43" t="s">
         <v>60</v>
       </c>
       <c r="C124" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D124" s="34" t="s">
+      <c r="D124" s="43" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="44"/>
-      <c r="B125" s="34"/>
+      <c r="A125" s="42"/>
+      <c r="B125" s="43"/>
       <c r="C125" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D125" s="34"/>
+      <c r="D125" s="43"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="44"/>
-      <c r="B126" s="34"/>
+      <c r="A126" s="42"/>
+      <c r="B126" s="43"/>
       <c r="C126" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D126" s="34"/>
+      <c r="D126" s="43"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="44"/>
-      <c r="B127" s="34"/>
+      <c r="A127" s="42"/>
+      <c r="B127" s="43"/>
       <c r="C127" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D127" s="34"/>
+      <c r="D127" s="43"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="44"/>
-      <c r="B128" s="34"/>
+      <c r="A128" s="42"/>
+      <c r="B128" s="43"/>
       <c r="C128" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D128" s="34"/>
+      <c r="D128" s="43"/>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="39" t="s">
+      <c r="A129" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="B129" s="36" t="s">
+      <c r="B129" s="45" t="s">
         <v>52</v>
       </c>
       <c r="C129" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D129" s="34" t="s">
+      <c r="D129" s="43" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="39"/>
-      <c r="B130" s="36"/>
+      <c r="A130" s="49"/>
+      <c r="B130" s="45"/>
       <c r="C130" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D130" s="34"/>
+      <c r="D130" s="43"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="39"/>
-      <c r="B131" s="36"/>
+      <c r="A131" s="49"/>
+      <c r="B131" s="45"/>
       <c r="C131" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D131" s="34"/>
+      <c r="D131" s="43"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="39"/>
-      <c r="B132" s="36"/>
+      <c r="A132" s="49"/>
+      <c r="B132" s="45"/>
       <c r="C132" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D132" s="34"/>
+      <c r="D132" s="43"/>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="40"/>
-      <c r="B133" s="37"/>
+      <c r="A133" s="50"/>
+      <c r="B133" s="46"/>
       <c r="C133" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D133" s="34"/>
+      <c r="D133" s="43"/>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="38" t="s">
+      <c r="A134" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="B134" s="35" t="s">
+      <c r="B134" s="44" t="s">
         <v>52</v>
       </c>
       <c r="C134" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D134" s="34" t="s">
+      <c r="D134" s="43" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="39"/>
-      <c r="B135" s="36"/>
+      <c r="A135" s="49"/>
+      <c r="B135" s="45"/>
       <c r="C135" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D135" s="34"/>
+      <c r="D135" s="43"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="39"/>
-      <c r="B136" s="36"/>
+      <c r="A136" s="49"/>
+      <c r="B136" s="45"/>
       <c r="C136" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D136" s="34"/>
+      <c r="D136" s="43"/>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="39"/>
-      <c r="B137" s="36"/>
+      <c r="A137" s="49"/>
+      <c r="B137" s="45"/>
       <c r="C137" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D137" s="34"/>
+      <c r="D137" s="43"/>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="40"/>
-      <c r="B138" s="37"/>
+      <c r="A138" s="50"/>
+      <c r="B138" s="46"/>
       <c r="C138" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D138" s="34"/>
+      <c r="D138" s="43"/>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="38" t="s">
+      <c r="A139" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="B139" s="35" t="s">
+      <c r="B139" s="44" t="s">
         <v>52</v>
       </c>
       <c r="C139" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D139" s="34" t="s">
+      <c r="D139" s="43" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="39"/>
-      <c r="B140" s="36"/>
+      <c r="A140" s="49"/>
+      <c r="B140" s="45"/>
       <c r="C140" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D140" s="34"/>
+      <c r="D140" s="43"/>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="39"/>
-      <c r="B141" s="36"/>
+      <c r="A141" s="49"/>
+      <c r="B141" s="45"/>
       <c r="C141" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D141" s="34"/>
+      <c r="D141" s="43"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="39"/>
-      <c r="B142" s="36"/>
+      <c r="A142" s="49"/>
+      <c r="B142" s="45"/>
       <c r="C142" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D142" s="34"/>
+      <c r="D142" s="43"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="40"/>
-      <c r="B143" s="37"/>
+      <c r="A143" s="50"/>
+      <c r="B143" s="46"/>
       <c r="C143" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D143" s="34"/>
+      <c r="D143" s="43"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="38" t="s">
+      <c r="A144" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="B144" s="35" t="s">
+      <c r="B144" s="44" t="s">
         <v>52</v>
       </c>
       <c r="C144" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D144" s="34" t="s">
+      <c r="D144" s="43" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="39"/>
-      <c r="B145" s="36"/>
+      <c r="A145" s="49"/>
+      <c r="B145" s="45"/>
       <c r="C145" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D145" s="34"/>
+      <c r="D145" s="43"/>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="39"/>
-      <c r="B146" s="36"/>
+      <c r="A146" s="49"/>
+      <c r="B146" s="45"/>
       <c r="C146" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D146" s="34"/>
+      <c r="D146" s="43"/>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="39"/>
-      <c r="B147" s="36"/>
+      <c r="A147" s="49"/>
+      <c r="B147" s="45"/>
       <c r="C147" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D147" s="34"/>
+      <c r="D147" s="43"/>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="40"/>
-      <c r="B148" s="37"/>
+      <c r="A148" s="50"/>
+      <c r="B148" s="46"/>
       <c r="C148" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D148" s="34"/>
+      <c r="D148" s="43"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="38" t="s">
+      <c r="A149" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="B149" s="35" t="s">
+      <c r="B149" s="44" t="s">
         <v>52</v>
       </c>
       <c r="C149" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D149" s="34" t="s">
+      <c r="D149" s="43" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="39"/>
-      <c r="B150" s="36"/>
+      <c r="A150" s="49"/>
+      <c r="B150" s="45"/>
       <c r="C150" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D150" s="34"/>
+      <c r="D150" s="43"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="39"/>
-      <c r="B151" s="36"/>
+      <c r="A151" s="49"/>
+      <c r="B151" s="45"/>
       <c r="C151" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D151" s="34"/>
+      <c r="D151" s="43"/>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="39"/>
-      <c r="B152" s="36"/>
+      <c r="A152" s="49"/>
+      <c r="B152" s="45"/>
       <c r="C152" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D152" s="34"/>
+      <c r="D152" s="43"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="40"/>
-      <c r="B153" s="37"/>
+      <c r="A153" s="50"/>
+      <c r="B153" s="46"/>
       <c r="C153" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D153" s="34"/>
+      <c r="D153" s="43"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="34" t="s">
+      <c r="A154" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="B154" s="34" t="s">
+      <c r="B154" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C154" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D154" s="34" t="s">
+      <c r="D154" s="43" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="34"/>
-      <c r="B155" s="34"/>
+      <c r="A155" s="43"/>
+      <c r="B155" s="43"/>
       <c r="C155" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D155" s="34"/>
+      <c r="D155" s="43"/>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="34"/>
-      <c r="B156" s="34"/>
+      <c r="A156" s="43"/>
+      <c r="B156" s="43"/>
       <c r="C156" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D156" s="34"/>
+      <c r="D156" s="43"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="34"/>
-      <c r="B157" s="34"/>
+      <c r="A157" s="43"/>
+      <c r="B157" s="43"/>
       <c r="C157" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="D157" s="34"/>
+      <c r="D157" s="43"/>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="34" t="s">
+      <c r="A158" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="B158" s="34" t="s">
+      <c r="B158" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C158" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D158" s="46" t="s">
+      <c r="D158" s="51" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="34"/>
-      <c r="B159" s="34"/>
+      <c r="A159" s="43"/>
+      <c r="B159" s="43"/>
       <c r="C159" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="D159" s="46"/>
+      <c r="D159" s="51"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="34"/>
-      <c r="B160" s="34"/>
+      <c r="A160" s="43"/>
+      <c r="B160" s="43"/>
       <c r="C160" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="D160" s="46"/>
+      <c r="D160" s="51"/>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="34"/>
-      <c r="B161" s="34"/>
+      <c r="A161" s="43"/>
+      <c r="B161" s="43"/>
       <c r="C161" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D161" s="46"/>
+      <c r="D161" s="51"/>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="34" t="s">
+      <c r="A162" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="B162" s="34" t="s">
+      <c r="B162" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C162" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D162" s="46" t="s">
+      <c r="D162" s="51" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="34"/>
-      <c r="B163" s="34"/>
+      <c r="A163" s="43"/>
+      <c r="B163" s="43"/>
       <c r="C163" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="D163" s="46"/>
+      <c r="D163" s="51"/>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="34"/>
-      <c r="B164" s="34"/>
+      <c r="A164" s="43"/>
+      <c r="B164" s="43"/>
       <c r="C164" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="D164" s="46"/>
+      <c r="D164" s="51"/>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="34"/>
-      <c r="B165" s="34"/>
+      <c r="A165" s="43"/>
+      <c r="B165" s="43"/>
       <c r="C165" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D165" s="46"/>
+      <c r="D165" s="51"/>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="34" t="s">
+      <c r="A166" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="B166" s="34" t="s">
+      <c r="B166" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C166" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D166" s="46" t="s">
+      <c r="D166" s="51" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="34"/>
-      <c r="B167" s="34"/>
+      <c r="A167" s="43"/>
+      <c r="B167" s="43"/>
       <c r="C167" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="D167" s="46"/>
+      <c r="D167" s="51"/>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="34"/>
-      <c r="B168" s="34"/>
+      <c r="A168" s="43"/>
+      <c r="B168" s="43"/>
       <c r="C168" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="D168" s="46"/>
+      <c r="D168" s="51"/>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="34"/>
-      <c r="B169" s="34"/>
+      <c r="A169" s="43"/>
+      <c r="B169" s="43"/>
       <c r="C169" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D169" s="46"/>
+      <c r="D169" s="51"/>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="34" t="s">
+      <c r="A170" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="B170" s="34" t="s">
+      <c r="B170" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C170" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D170" s="46" t="s">
+      <c r="D170" s="51" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="34"/>
-      <c r="B171" s="34"/>
+      <c r="A171" s="43"/>
+      <c r="B171" s="43"/>
       <c r="C171" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="D171" s="46"/>
+      <c r="D171" s="51"/>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="34"/>
-      <c r="B172" s="34"/>
+      <c r="A172" s="43"/>
+      <c r="B172" s="43"/>
       <c r="C172" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="D172" s="46"/>
+      <c r="D172" s="51"/>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="34"/>
-      <c r="B173" s="34"/>
+      <c r="A173" s="43"/>
+      <c r="B173" s="43"/>
       <c r="C173" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D173" s="46"/>
+      <c r="D173" s="51"/>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="34" t="s">
+      <c r="A174" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="B174" s="34" t="s">
+      <c r="B174" s="43" t="s">
         <v>79</v>
       </c>
       <c r="C174" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D174" s="34" t="s">
+      <c r="D174" s="43" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="34"/>
-      <c r="B175" s="34"/>
+      <c r="A175" s="43"/>
+      <c r="B175" s="43"/>
       <c r="C175" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D175" s="34"/>
+      <c r="D175" s="43"/>
     </row>
     <row r="176" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A176" s="34"/>
-      <c r="B176" s="34"/>
+      <c r="A176" s="43"/>
+      <c r="B176" s="43"/>
       <c r="C176" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D176" s="34"/>
+      <c r="D176" s="43"/>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="34"/>
-      <c r="B177" s="34"/>
+      <c r="A177" s="43"/>
+      <c r="B177" s="43"/>
       <c r="C177" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D177" s="34"/>
+      <c r="D177" s="43"/>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="34" t="s">
+      <c r="A178" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="B178" s="34" t="s">
+      <c r="B178" s="43" t="s">
         <v>79</v>
       </c>
       <c r="C178" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D178" s="34" t="s">
+      <c r="D178" s="43" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="34"/>
-      <c r="B179" s="34"/>
+      <c r="A179" s="43"/>
+      <c r="B179" s="43"/>
       <c r="C179" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D179" s="34"/>
+      <c r="D179" s="43"/>
     </row>
     <row r="180" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A180" s="34"/>
-      <c r="B180" s="34"/>
+      <c r="A180" s="43"/>
+      <c r="B180" s="43"/>
       <c r="C180" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D180" s="34"/>
+      <c r="D180" s="43"/>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="34"/>
-      <c r="B181" s="34"/>
+      <c r="A181" s="43"/>
+      <c r="B181" s="43"/>
       <c r="C181" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D181" s="34"/>
+      <c r="D181" s="43"/>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="34" t="s">
+      <c r="A182" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="B182" s="34" t="s">
+      <c r="B182" s="43" t="s">
         <v>79</v>
       </c>
       <c r="C182" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D182" s="34" t="s">
+      <c r="D182" s="43" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="34"/>
-      <c r="B183" s="34"/>
+      <c r="A183" s="43"/>
+      <c r="B183" s="43"/>
       <c r="C183" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D183" s="34"/>
+      <c r="D183" s="43"/>
     </row>
     <row r="184" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A184" s="34"/>
-      <c r="B184" s="34"/>
+      <c r="A184" s="43"/>
+      <c r="B184" s="43"/>
       <c r="C184" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D184" s="34"/>
+      <c r="D184" s="43"/>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="34"/>
-      <c r="B185" s="34"/>
+      <c r="A185" s="43"/>
+      <c r="B185" s="43"/>
       <c r="C185" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D185" s="34"/>
+      <c r="D185" s="43"/>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="34" t="s">
+      <c r="A186" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="B186" s="34" t="s">
+      <c r="B186" s="43" t="s">
         <v>88</v>
       </c>
       <c r="C186" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D186" s="45" t="s">
+      <c r="D186" s="52" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" s="34"/>
-      <c r="B187" s="34"/>
+      <c r="A187" s="43"/>
+      <c r="B187" s="43"/>
       <c r="C187" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D187" s="45"/>
+      <c r="D187" s="52"/>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="34"/>
-      <c r="B188" s="34"/>
+      <c r="A188" s="43"/>
+      <c r="B188" s="43"/>
       <c r="C188" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D188" s="45"/>
+      <c r="D188" s="52"/>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="44" t="s">
+      <c r="A189" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="B189" s="34" t="s">
+      <c r="B189" s="43" t="s">
         <v>88</v>
       </c>
       <c r="C189" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D189" s="45" t="s">
+      <c r="D189" s="52" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="44"/>
-      <c r="B190" s="34"/>
+      <c r="A190" s="42"/>
+      <c r="B190" s="43"/>
       <c r="C190" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D190" s="45"/>
+      <c r="D190" s="52"/>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" s="44"/>
-      <c r="B191" s="34"/>
+      <c r="A191" s="42"/>
+      <c r="B191" s="43"/>
       <c r="C191" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D191" s="45"/>
+      <c r="D191" s="52"/>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="44"/>
-      <c r="B192" s="34"/>
+      <c r="A192" s="42"/>
+      <c r="B192" s="43"/>
       <c r="C192" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D192" s="45"/>
+      <c r="D192" s="52"/>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" s="38" t="s">
+      <c r="A193" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="B193" s="35" t="s">
+      <c r="B193" s="44" t="s">
         <v>88</v>
       </c>
       <c r="C193" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D193" s="41" t="s">
+      <c r="D193" s="53" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="39"/>
-      <c r="B194" s="36"/>
+      <c r="A194" s="49"/>
+      <c r="B194" s="45"/>
       <c r="C194" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D194" s="42"/>
+      <c r="D194" s="54"/>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="39"/>
-      <c r="B195" s="36"/>
+      <c r="A195" s="49"/>
+      <c r="B195" s="45"/>
       <c r="C195" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D195" s="42"/>
+      <c r="D195" s="54"/>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" s="39"/>
-      <c r="B196" s="36"/>
+      <c r="A196" s="49"/>
+      <c r="B196" s="45"/>
       <c r="C196" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D196" s="42"/>
+      <c r="D196" s="54"/>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="39"/>
-      <c r="B197" s="36"/>
+      <c r="A197" s="49"/>
+      <c r="B197" s="45"/>
       <c r="C197" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D197" s="42"/>
+      <c r="D197" s="54"/>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="39"/>
-      <c r="B198" s="36"/>
+      <c r="A198" s="49"/>
+      <c r="B198" s="45"/>
       <c r="C198" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="D198" s="42"/>
+      <c r="D198" s="54"/>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="39"/>
-      <c r="B199" s="36"/>
+      <c r="A199" s="49"/>
+      <c r="B199" s="45"/>
       <c r="C199" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D199" s="42"/>
+      <c r="D199" s="54"/>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="39"/>
-      <c r="B200" s="36"/>
+      <c r="A200" s="49"/>
+      <c r="B200" s="45"/>
       <c r="C200" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D200" s="42"/>
+      <c r="D200" s="54"/>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="40"/>
-      <c r="B201" s="37"/>
+      <c r="A201" s="50"/>
+      <c r="B201" s="46"/>
       <c r="C201" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="D201" s="43"/>
+      <c r="D201" s="55"/>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="38" t="s">
+      <c r="A202" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="B202" s="35" t="s">
+      <c r="B202" s="44" t="s">
         <v>88</v>
       </c>
       <c r="C202" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D202" s="41" t="s">
+      <c r="D202" s="53" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="39"/>
-      <c r="B203" s="36"/>
+      <c r="A203" s="49"/>
+      <c r="B203" s="45"/>
       <c r="C203" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D203" s="42"/>
+      <c r="D203" s="54"/>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="39"/>
-      <c r="B204" s="36"/>
+      <c r="A204" s="49"/>
+      <c r="B204" s="45"/>
       <c r="C204" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D204" s="42"/>
+      <c r="D204" s="54"/>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="39"/>
-      <c r="B205" s="36"/>
+      <c r="A205" s="49"/>
+      <c r="B205" s="45"/>
       <c r="C205" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D205" s="42"/>
+      <c r="D205" s="54"/>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206" s="39"/>
-      <c r="B206" s="36"/>
+      <c r="A206" s="49"/>
+      <c r="B206" s="45"/>
       <c r="C206" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D206" s="42"/>
+      <c r="D206" s="54"/>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" s="39"/>
-      <c r="B207" s="36"/>
+      <c r="A207" s="49"/>
+      <c r="B207" s="45"/>
       <c r="C207" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="D207" s="42"/>
+      <c r="D207" s="54"/>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" s="39"/>
-      <c r="B208" s="36"/>
+      <c r="A208" s="49"/>
+      <c r="B208" s="45"/>
       <c r="C208" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D208" s="42"/>
+      <c r="D208" s="54"/>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A209" s="39"/>
-      <c r="B209" s="36"/>
+      <c r="A209" s="49"/>
+      <c r="B209" s="45"/>
       <c r="C209" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D209" s="42"/>
+      <c r="D209" s="54"/>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A210" s="40"/>
-      <c r="B210" s="37"/>
+      <c r="A210" s="50"/>
+      <c r="B210" s="46"/>
       <c r="C210" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="D210" s="43"/>
+      <c r="D210" s="55"/>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A211" s="38" t="s">
+      <c r="A211" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="B211" s="35" t="s">
+      <c r="B211" s="44" t="s">
         <v>88</v>
       </c>
       <c r="C211" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D211" s="41" t="s">
+      <c r="D211" s="53" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A212" s="39"/>
-      <c r="B212" s="36"/>
+      <c r="A212" s="49"/>
+      <c r="B212" s="45"/>
       <c r="C212" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D212" s="42"/>
+      <c r="D212" s="54"/>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A213" s="39"/>
-      <c r="B213" s="36"/>
+      <c r="A213" s="49"/>
+      <c r="B213" s="45"/>
       <c r="C213" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D213" s="42"/>
+      <c r="D213" s="54"/>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A214" s="39"/>
-      <c r="B214" s="36"/>
+      <c r="A214" s="49"/>
+      <c r="B214" s="45"/>
       <c r="C214" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D214" s="42"/>
+      <c r="D214" s="54"/>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A215" s="39"/>
-      <c r="B215" s="36"/>
+      <c r="A215" s="49"/>
+      <c r="B215" s="45"/>
       <c r="C215" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="D215" s="42"/>
+      <c r="D215" s="54"/>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A216" s="39"/>
-      <c r="B216" s="36"/>
+      <c r="A216" s="49"/>
+      <c r="B216" s="45"/>
       <c r="C216" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D216" s="42"/>
+      <c r="D216" s="54"/>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A217" s="39"/>
-      <c r="B217" s="36"/>
+      <c r="A217" s="49"/>
+      <c r="B217" s="45"/>
       <c r="C217" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="D217" s="42"/>
+      <c r="D217" s="54"/>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A218" s="39"/>
-      <c r="B218" s="36"/>
+      <c r="A218" s="49"/>
+      <c r="B218" s="45"/>
       <c r="C218" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D218" s="42"/>
+      <c r="D218" s="54"/>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A219" s="40"/>
-      <c r="B219" s="37"/>
+      <c r="A219" s="50"/>
+      <c r="B219" s="46"/>
       <c r="C219" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="D219" s="43"/>
+      <c r="D219" s="55"/>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A220" s="38" t="s">
+      <c r="A220" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="B220" s="35" t="s">
+      <c r="B220" s="44" t="s">
         <v>88</v>
       </c>
       <c r="C220" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D220" s="41" t="s">
+      <c r="D220" s="53" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A221" s="39"/>
-      <c r="B221" s="36"/>
+      <c r="A221" s="49"/>
+      <c r="B221" s="45"/>
       <c r="C221" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D221" s="42"/>
+      <c r="D221" s="54"/>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A222" s="39"/>
-      <c r="B222" s="36"/>
+      <c r="A222" s="49"/>
+      <c r="B222" s="45"/>
       <c r="C222" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D222" s="42"/>
+      <c r="D222" s="54"/>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A223" s="39"/>
-      <c r="B223" s="36"/>
+      <c r="A223" s="49"/>
+      <c r="B223" s="45"/>
       <c r="C223" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D223" s="42"/>
+      <c r="D223" s="54"/>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A224" s="39"/>
-      <c r="B224" s="36"/>
+      <c r="A224" s="49"/>
+      <c r="B224" s="45"/>
       <c r="C224" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D224" s="42"/>
+      <c r="D224" s="54"/>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A225" s="39"/>
-      <c r="B225" s="36"/>
+      <c r="A225" s="49"/>
+      <c r="B225" s="45"/>
       <c r="C225" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="D225" s="42"/>
+      <c r="D225" s="54"/>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A226" s="39"/>
-      <c r="B226" s="36"/>
+      <c r="A226" s="49"/>
+      <c r="B226" s="45"/>
       <c r="C226" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="D226" s="42"/>
+      <c r="D226" s="54"/>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A227" s="39"/>
-      <c r="B227" s="36"/>
+      <c r="A227" s="49"/>
+      <c r="B227" s="45"/>
       <c r="C227" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="D227" s="42"/>
+      <c r="D227" s="54"/>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A228" s="40"/>
-      <c r="B228" s="37"/>
+      <c r="A228" s="50"/>
+      <c r="B228" s="46"/>
       <c r="C228" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="D228" s="43"/>
+      <c r="D228" s="55"/>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A229" s="34" t="s">
+      <c r="A229" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="B229" s="34" t="s">
+      <c r="B229" s="43" t="s">
         <v>118</v>
       </c>
       <c r="C229" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D229" s="35" t="s">
+      <c r="D229" s="44" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A230" s="34"/>
-      <c r="B230" s="34"/>
+      <c r="A230" s="43"/>
+      <c r="B230" s="43"/>
       <c r="C230" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D230" s="36"/>
+      <c r="D230" s="45"/>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A231" s="34"/>
-      <c r="B231" s="34"/>
+      <c r="A231" s="43"/>
+      <c r="B231" s="43"/>
       <c r="C231" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D231" s="36"/>
+      <c r="D231" s="45"/>
     </row>
     <row r="232" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A232" s="34"/>
-      <c r="B232" s="34"/>
+      <c r="A232" s="43"/>
+      <c r="B232" s="43"/>
       <c r="C232" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D232" s="36"/>
+      <c r="D232" s="45"/>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" s="34"/>
-      <c r="B233" s="34"/>
+      <c r="A233" s="43"/>
+      <c r="B233" s="43"/>
       <c r="C233" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D233" s="37"/>
+      <c r="D233" s="46"/>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234" s="34" t="s">
+      <c r="A234" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="B234" s="34" t="s">
+      <c r="B234" s="43" t="s">
         <v>118</v>
       </c>
       <c r="C234" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D234" s="35" t="s">
+      <c r="D234" s="44" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A235" s="34"/>
-      <c r="B235" s="34"/>
+      <c r="A235" s="43"/>
+      <c r="B235" s="43"/>
       <c r="C235" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D235" s="36"/>
+      <c r="D235" s="45"/>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A236" s="34"/>
-      <c r="B236" s="34"/>
+      <c r="A236" s="43"/>
+      <c r="B236" s="43"/>
       <c r="C236" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D236" s="36"/>
+      <c r="D236" s="45"/>
     </row>
     <row r="237" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A237" s="34"/>
-      <c r="B237" s="34"/>
+      <c r="A237" s="43"/>
+      <c r="B237" s="43"/>
       <c r="C237" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="D237" s="36"/>
+      <c r="D237" s="45"/>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A238" s="34"/>
-      <c r="B238" s="34"/>
+      <c r="A238" s="43"/>
+      <c r="B238" s="43"/>
       <c r="C238" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D238" s="37"/>
+      <c r="D238" s="46"/>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A239" s="34" t="s">
+      <c r="A239" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="B239" s="34" t="s">
+      <c r="B239" s="43" t="s">
         <v>118</v>
       </c>
       <c r="C239" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D239" s="35" t="s">
+      <c r="D239" s="44" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A240" s="34"/>
-      <c r="B240" s="34"/>
+      <c r="A240" s="43"/>
+      <c r="B240" s="43"/>
       <c r="C240" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D240" s="36"/>
+      <c r="D240" s="45"/>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A241" s="34"/>
-      <c r="B241" s="34"/>
+      <c r="A241" s="43"/>
+      <c r="B241" s="43"/>
       <c r="C241" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D241" s="36"/>
+      <c r="D241" s="45"/>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A242" s="34"/>
-      <c r="B242" s="34"/>
+      <c r="A242" s="43"/>
+      <c r="B242" s="43"/>
       <c r="C242" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="D242" s="36"/>
+      <c r="D242" s="45"/>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A243" s="34"/>
-      <c r="B243" s="34"/>
+      <c r="A243" s="43"/>
+      <c r="B243" s="43"/>
       <c r="C243" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D243" s="37"/>
+      <c r="D243" s="46"/>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" s="2"/>
@@ -3521,6 +3572,138 @@
     </row>
   </sheetData>
   <mergeCells count="145">
+    <mergeCell ref="A234:A238"/>
+    <mergeCell ref="B234:B238"/>
+    <mergeCell ref="D234:D238"/>
+    <mergeCell ref="A239:A243"/>
+    <mergeCell ref="B239:B243"/>
+    <mergeCell ref="D239:D243"/>
+    <mergeCell ref="A220:A228"/>
+    <mergeCell ref="B220:B228"/>
+    <mergeCell ref="D220:D228"/>
+    <mergeCell ref="A229:A233"/>
+    <mergeCell ref="B229:B233"/>
+    <mergeCell ref="D229:D233"/>
+    <mergeCell ref="A202:A210"/>
+    <mergeCell ref="B202:B210"/>
+    <mergeCell ref="D202:D210"/>
+    <mergeCell ref="A211:A219"/>
+    <mergeCell ref="B211:B219"/>
+    <mergeCell ref="D211:D219"/>
+    <mergeCell ref="A189:A192"/>
+    <mergeCell ref="B189:B192"/>
+    <mergeCell ref="D189:D192"/>
+    <mergeCell ref="A193:A201"/>
+    <mergeCell ref="B193:B201"/>
+    <mergeCell ref="D193:D201"/>
+    <mergeCell ref="A182:A185"/>
+    <mergeCell ref="B182:B185"/>
+    <mergeCell ref="D182:D185"/>
+    <mergeCell ref="A186:A188"/>
+    <mergeCell ref="B186:B188"/>
+    <mergeCell ref="D186:D188"/>
+    <mergeCell ref="A174:A177"/>
+    <mergeCell ref="B174:B177"/>
+    <mergeCell ref="D174:D177"/>
+    <mergeCell ref="A178:A181"/>
+    <mergeCell ref="B178:B181"/>
+    <mergeCell ref="D178:D181"/>
+    <mergeCell ref="A166:A169"/>
+    <mergeCell ref="B166:B169"/>
+    <mergeCell ref="D166:D169"/>
+    <mergeCell ref="A170:A173"/>
+    <mergeCell ref="B170:B173"/>
+    <mergeCell ref="D170:D173"/>
+    <mergeCell ref="A158:A161"/>
+    <mergeCell ref="B158:B161"/>
+    <mergeCell ref="D158:D161"/>
+    <mergeCell ref="A162:A165"/>
+    <mergeCell ref="B162:B165"/>
+    <mergeCell ref="D162:D165"/>
+    <mergeCell ref="A149:A153"/>
+    <mergeCell ref="B149:B153"/>
+    <mergeCell ref="D149:D153"/>
+    <mergeCell ref="A154:A157"/>
+    <mergeCell ref="B154:B157"/>
+    <mergeCell ref="D154:D157"/>
+    <mergeCell ref="A139:A143"/>
+    <mergeCell ref="B139:B143"/>
+    <mergeCell ref="D139:D143"/>
+    <mergeCell ref="A144:A148"/>
+    <mergeCell ref="B144:B148"/>
+    <mergeCell ref="D144:D148"/>
+    <mergeCell ref="A129:A133"/>
+    <mergeCell ref="B129:B133"/>
+    <mergeCell ref="D129:D133"/>
+    <mergeCell ref="A134:A138"/>
+    <mergeCell ref="B134:B138"/>
+    <mergeCell ref="D134:D138"/>
+    <mergeCell ref="A119:A123"/>
+    <mergeCell ref="B119:B123"/>
+    <mergeCell ref="D119:D123"/>
+    <mergeCell ref="A124:A128"/>
+    <mergeCell ref="B124:B128"/>
+    <mergeCell ref="D124:D128"/>
+    <mergeCell ref="A109:A113"/>
+    <mergeCell ref="B109:B113"/>
+    <mergeCell ref="D109:D113"/>
+    <mergeCell ref="A114:A118"/>
+    <mergeCell ref="B114:B118"/>
+    <mergeCell ref="D114:D118"/>
+    <mergeCell ref="A99:A103"/>
+    <mergeCell ref="B99:B103"/>
+    <mergeCell ref="D99:D103"/>
+    <mergeCell ref="A104:A108"/>
+    <mergeCell ref="B104:B108"/>
+    <mergeCell ref="D104:D108"/>
+    <mergeCell ref="A89:A93"/>
+    <mergeCell ref="B89:B93"/>
+    <mergeCell ref="D89:D93"/>
+    <mergeCell ref="A94:A98"/>
+    <mergeCell ref="B94:B98"/>
+    <mergeCell ref="D94:D98"/>
+    <mergeCell ref="A79:A83"/>
+    <mergeCell ref="B79:B83"/>
+    <mergeCell ref="D79:D83"/>
+    <mergeCell ref="A84:A88"/>
+    <mergeCell ref="B84:B88"/>
+    <mergeCell ref="D84:D88"/>
+    <mergeCell ref="A69:A73"/>
+    <mergeCell ref="B69:B73"/>
+    <mergeCell ref="D69:D73"/>
+    <mergeCell ref="A74:A78"/>
+    <mergeCell ref="B74:B78"/>
+    <mergeCell ref="D74:D78"/>
+    <mergeCell ref="A59:A63"/>
+    <mergeCell ref="B59:B63"/>
+    <mergeCell ref="D59:D63"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="B64:B68"/>
+    <mergeCell ref="D64:D68"/>
+    <mergeCell ref="A50:A54"/>
+    <mergeCell ref="B50:B54"/>
+    <mergeCell ref="D50:D54"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="D55:D58"/>
+    <mergeCell ref="A41:A45"/>
+    <mergeCell ref="B41:B45"/>
+    <mergeCell ref="D41:D45"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="D46:D49"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="D32:D36"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="D37:D40"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="D23:D27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="D28:D31"/>
     <mergeCell ref="A14:A18"/>
     <mergeCell ref="B14:B18"/>
     <mergeCell ref="D14:D18"/>
@@ -3534,138 +3717,6 @@
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="D10:D13"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="D32:D36"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="D37:D40"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="D23:D27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="A50:A54"/>
-    <mergeCell ref="B50:B54"/>
-    <mergeCell ref="D50:D54"/>
-    <mergeCell ref="A55:A58"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="D55:D58"/>
-    <mergeCell ref="A41:A45"/>
-    <mergeCell ref="B41:B45"/>
-    <mergeCell ref="D41:D45"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="D46:D49"/>
-    <mergeCell ref="A69:A73"/>
-    <mergeCell ref="B69:B73"/>
-    <mergeCell ref="D69:D73"/>
-    <mergeCell ref="A74:A78"/>
-    <mergeCell ref="B74:B78"/>
-    <mergeCell ref="D74:D78"/>
-    <mergeCell ref="A59:A63"/>
-    <mergeCell ref="B59:B63"/>
-    <mergeCell ref="D59:D63"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="B64:B68"/>
-    <mergeCell ref="D64:D68"/>
-    <mergeCell ref="A89:A93"/>
-    <mergeCell ref="B89:B93"/>
-    <mergeCell ref="D89:D93"/>
-    <mergeCell ref="A94:A98"/>
-    <mergeCell ref="B94:B98"/>
-    <mergeCell ref="D94:D98"/>
-    <mergeCell ref="A79:A83"/>
-    <mergeCell ref="B79:B83"/>
-    <mergeCell ref="D79:D83"/>
-    <mergeCell ref="A84:A88"/>
-    <mergeCell ref="B84:B88"/>
-    <mergeCell ref="D84:D88"/>
-    <mergeCell ref="A109:A113"/>
-    <mergeCell ref="B109:B113"/>
-    <mergeCell ref="D109:D113"/>
-    <mergeCell ref="A114:A118"/>
-    <mergeCell ref="B114:B118"/>
-    <mergeCell ref="D114:D118"/>
-    <mergeCell ref="A99:A103"/>
-    <mergeCell ref="B99:B103"/>
-    <mergeCell ref="D99:D103"/>
-    <mergeCell ref="A104:A108"/>
-    <mergeCell ref="B104:B108"/>
-    <mergeCell ref="D104:D108"/>
-    <mergeCell ref="A129:A133"/>
-    <mergeCell ref="B129:B133"/>
-    <mergeCell ref="D129:D133"/>
-    <mergeCell ref="A134:A138"/>
-    <mergeCell ref="B134:B138"/>
-    <mergeCell ref="D134:D138"/>
-    <mergeCell ref="A119:A123"/>
-    <mergeCell ref="B119:B123"/>
-    <mergeCell ref="D119:D123"/>
-    <mergeCell ref="A124:A128"/>
-    <mergeCell ref="B124:B128"/>
-    <mergeCell ref="D124:D128"/>
-    <mergeCell ref="A149:A153"/>
-    <mergeCell ref="B149:B153"/>
-    <mergeCell ref="D149:D153"/>
-    <mergeCell ref="A154:A157"/>
-    <mergeCell ref="B154:B157"/>
-    <mergeCell ref="D154:D157"/>
-    <mergeCell ref="A139:A143"/>
-    <mergeCell ref="B139:B143"/>
-    <mergeCell ref="D139:D143"/>
-    <mergeCell ref="A144:A148"/>
-    <mergeCell ref="B144:B148"/>
-    <mergeCell ref="D144:D148"/>
-    <mergeCell ref="A166:A169"/>
-    <mergeCell ref="B166:B169"/>
-    <mergeCell ref="D166:D169"/>
-    <mergeCell ref="A170:A173"/>
-    <mergeCell ref="B170:B173"/>
-    <mergeCell ref="D170:D173"/>
-    <mergeCell ref="A158:A161"/>
-    <mergeCell ref="B158:B161"/>
-    <mergeCell ref="D158:D161"/>
-    <mergeCell ref="A162:A165"/>
-    <mergeCell ref="B162:B165"/>
-    <mergeCell ref="D162:D165"/>
-    <mergeCell ref="A182:A185"/>
-    <mergeCell ref="B182:B185"/>
-    <mergeCell ref="D182:D185"/>
-    <mergeCell ref="A186:A188"/>
-    <mergeCell ref="B186:B188"/>
-    <mergeCell ref="D186:D188"/>
-    <mergeCell ref="A174:A177"/>
-    <mergeCell ref="B174:B177"/>
-    <mergeCell ref="D174:D177"/>
-    <mergeCell ref="A178:A181"/>
-    <mergeCell ref="B178:B181"/>
-    <mergeCell ref="D178:D181"/>
-    <mergeCell ref="A202:A210"/>
-    <mergeCell ref="B202:B210"/>
-    <mergeCell ref="D202:D210"/>
-    <mergeCell ref="A211:A219"/>
-    <mergeCell ref="B211:B219"/>
-    <mergeCell ref="D211:D219"/>
-    <mergeCell ref="A189:A192"/>
-    <mergeCell ref="B189:B192"/>
-    <mergeCell ref="D189:D192"/>
-    <mergeCell ref="A193:A201"/>
-    <mergeCell ref="B193:B201"/>
-    <mergeCell ref="D193:D201"/>
-    <mergeCell ref="A234:A238"/>
-    <mergeCell ref="B234:B238"/>
-    <mergeCell ref="D234:D238"/>
-    <mergeCell ref="A239:A243"/>
-    <mergeCell ref="B239:B243"/>
-    <mergeCell ref="D239:D243"/>
-    <mergeCell ref="A220:A228"/>
-    <mergeCell ref="B220:B228"/>
-    <mergeCell ref="D220:D228"/>
-    <mergeCell ref="A229:A233"/>
-    <mergeCell ref="B229:B233"/>
-    <mergeCell ref="D229:D233"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3677,7 +3728,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D4" sqref="A2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4357,16 +4408,16 @@
       </c>
     </row>
     <row r="3" spans="1:9" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="22">
+      <c r="A3" s="56">
         <v>1</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="56" t="s">
         <v>138</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="56" t="s">
         <v>139</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="56" t="s">
         <v>140</v>
       </c>
       <c r="E3" s="22" t="s">
@@ -4383,16 +4434,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="22">
+      <c r="A4" s="56">
         <v>2</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="56" t="s">
         <v>138</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="56" t="s">
         <v>144</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="56" t="s">
         <v>145</v>
       </c>
       <c r="E4" s="22" t="s">
@@ -4735,4 +4786,283 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" style="57" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="57" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="72.42578125" style="57" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="57" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="57" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="57"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="58" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="58" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="58" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="58" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="58" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="59">
+        <v>1</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>183</v>
+      </c>
+      <c r="D2" s="59" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" s="60">
+        <v>42670</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="59">
+        <v>2</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>184</v>
+      </c>
+      <c r="D3" s="59" t="s">
+        <v>141</v>
+      </c>
+      <c r="E3" s="60">
+        <v>42670</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="61">
+        <v>3</v>
+      </c>
+      <c r="B4" s="61" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" s="61" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" s="61" t="s">
+        <v>141</v>
+      </c>
+      <c r="E4" s="62">
+        <v>42700</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="61">
+        <v>4</v>
+      </c>
+      <c r="B5" s="61" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" s="61" t="s">
+        <v>151</v>
+      </c>
+      <c r="D5" s="61" t="s">
+        <v>141</v>
+      </c>
+      <c r="E5" s="62">
+        <v>42700</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="61">
+        <v>5</v>
+      </c>
+      <c r="B6" s="61" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="61" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" s="61" t="s">
+        <v>141</v>
+      </c>
+      <c r="E6" s="62">
+        <v>42700</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="59">
+        <v>6</v>
+      </c>
+      <c r="B7" s="59" t="s">
+        <v>138</v>
+      </c>
+      <c r="C7" s="59" t="s">
+        <v>156</v>
+      </c>
+      <c r="D7" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="E7" s="60">
+        <v>42700</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="61">
+        <v>8</v>
+      </c>
+      <c r="B8" s="61" t="s">
+        <v>160</v>
+      </c>
+      <c r="C8" s="61" t="s">
+        <v>161</v>
+      </c>
+      <c r="D8" s="61" t="s">
+        <v>163</v>
+      </c>
+      <c r="E8" s="62">
+        <v>42700</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="59">
+        <v>13</v>
+      </c>
+      <c r="B9" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="C9" s="59" t="s">
+        <v>167</v>
+      </c>
+      <c r="D9" s="59" t="s">
+        <v>163</v>
+      </c>
+      <c r="E9" s="60">
+        <v>42700</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="59">
+        <v>14</v>
+      </c>
+      <c r="B10" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="C10" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="D10" s="59" t="s">
+        <v>163</v>
+      </c>
+      <c r="E10" s="60">
+        <v>42700</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="63">
+        <v>7</v>
+      </c>
+      <c r="B11" s="63" t="s">
+        <v>138</v>
+      </c>
+      <c r="C11" s="63" t="s">
+        <v>171</v>
+      </c>
+      <c r="D11" s="63" t="s">
+        <v>158</v>
+      </c>
+      <c r="E11" s="64">
+        <v>42700</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="63">
+        <v>9</v>
+      </c>
+      <c r="B12" s="63" t="s">
+        <v>160</v>
+      </c>
+      <c r="C12" s="63" t="s">
+        <v>174</v>
+      </c>
+      <c r="D12" s="63" t="s">
+        <v>163</v>
+      </c>
+      <c r="E12" s="64">
+        <v>42700</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="63">
+        <v>10</v>
+      </c>
+      <c r="B13" s="63" t="s">
+        <v>160</v>
+      </c>
+      <c r="C13" s="63" t="s">
+        <v>176</v>
+      </c>
+      <c r="D13" s="63" t="s">
+        <v>163</v>
+      </c>
+      <c r="E13" s="64">
+        <v>42700</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="63">
+        <v>11</v>
+      </c>
+      <c r="B14" s="63" t="s">
+        <v>160</v>
+      </c>
+      <c r="C14" s="63" t="s">
+        <v>178</v>
+      </c>
+      <c r="D14" s="63" t="s">
+        <v>163</v>
+      </c>
+      <c r="E14" s="64">
+        <v>42700</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="63">
+        <v>12</v>
+      </c>
+      <c r="B15" s="63" t="s">
+        <v>160</v>
+      </c>
+      <c r="C15" s="63" t="s">
+        <v>180</v>
+      </c>
+      <c r="D15" s="63" t="s">
+        <v>163</v>
+      </c>
+      <c r="E15" s="64">
+        <v>42700</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>